<commit_message>
Fixing some bugs in the plots and report format.  updating example data
</commit_message>
<xml_diff>
--- a/example/endoscopy.xlsx
+++ b/example/endoscopy.xlsx
@@ -1,31 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skillcoy/workspace/barrettsprogressionrisk/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C7ED62-6AA0-E848-AA6C-A2AB3270D570}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{594EBDF2-7CE6-0149-8C58-6074B1820C76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10360" yWindow="4160" windowWidth="28040" windowHeight="17440" xr2:uid="{FB7256DB-7A12-E94F-9FC0-C34B41B4EF31}"/>
+    <workbookView xWindow="7700" yWindow="8660" windowWidth="27240" windowHeight="16440" xr2:uid="{BF7BB43F-A71A-3F40-B0C7-FE16819DD8DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+  <si>
+    <t>LGD</t>
+  </si>
+  <si>
+    <t>HGD</t>
+  </si>
   <si>
     <t>Sample</t>
   </si>
@@ -33,28 +45,34 @@
     <t>Endoscopy</t>
   </si>
   <si>
-    <t>Sample.A</t>
-  </si>
-  <si>
-    <t>Sample.B</t>
-  </si>
-  <si>
-    <t>Sample.C</t>
-  </si>
-  <si>
-    <t>GEJ.Distance</t>
+    <t>Pathology</t>
+  </si>
+  <si>
+    <t>NDBE</t>
   </si>
   <si>
     <t>p53 IHC</t>
   </si>
   <si>
-    <t>NDBE</t>
-  </si>
-  <si>
-    <t>LGD</t>
-  </si>
-  <si>
-    <t>pathology</t>
+    <t>GEJ Distance</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -62,12 +80,34 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -93,9 +133,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,84 +464,137 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F86111-6822-6B49-A495-CD0A3A5317FD}">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE36ECCF-B24B-4549-95FE-268FA200490C}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4">
+        <v>39096</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4">
+        <v>39255</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4">
+        <v>39255</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E4" s="5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4">
+        <v>39390</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4">
+        <v>39390</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1">
-        <v>43154</v>
-      </c>
-      <c r="C2">
-        <v>28</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2">
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="4">
+        <v>39390</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1">
-        <v>43154</v>
-      </c>
-      <c r="C3">
+      <c r="E7" s="5">
         <v>34</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>43403</v>
-      </c>
-      <c r="C4">
-        <v>28</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>